<commit_message>
iC3_field_School_2024 modified and processed, plots and RBR data added, as well as Last station profile modified.
</commit_message>
<xml_diff>
--- a/iC3_field_school_2024/scripts/python/notebooks/inspect/Bottle_averages_CTD.xlsx
+++ b/iC3_field_school_2024/scripts/python/notebooks/inspect/Bottle_averages_CTD.xlsx
@@ -506,8 +506,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>72</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>343</v>
@@ -526,8 +528,10 @@
       <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>72</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>50</v>
@@ -562,8 +566,10 @@
       <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>72</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>20</v>
@@ -598,8 +604,10 @@
       <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>72</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -634,8 +642,10 @@
       <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>72</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>25</v>
@@ -670,8 +680,10 @@
       <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>74</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>54</v>
@@ -706,8 +718,10 @@
       <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>74</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>40</v>
@@ -742,8 +756,10 @@
       <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>74</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>20</v>
@@ -778,8 +794,10 @@
       <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>74</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>10</v>
@@ -814,8 +832,10 @@
       <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>74</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>2</v>
@@ -850,8 +870,10 @@
       <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>74</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
       </c>
       <c r="B12" t="n">
         <v>25</v>
@@ -886,8 +908,10 @@
       <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>83</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
       </c>
       <c r="B13" t="n">
         <v>116.5</v>
@@ -906,8 +930,10 @@
       <c r="N13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>83</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
       </c>
       <c r="B14" t="n">
         <v>50</v>
@@ -942,8 +968,10 @@
       <c r="N14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>83</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
       </c>
       <c r="B15" t="n">
         <v>20</v>
@@ -978,8 +1006,10 @@
       <c r="N15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>83</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
       </c>
       <c r="B16" t="n">
         <v>10</v>
@@ -1014,8 +1044,10 @@
       <c r="N16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>83</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
       </c>
       <c r="B17" t="n">
         <v>2</v>
@@ -1050,8 +1082,10 @@
       <c r="N17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>83</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
       </c>
       <c r="B18" t="n">
         <v>25</v>
@@ -1086,8 +1120,10 @@
       <c r="N18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>95</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
       </c>
       <c r="B19" t="n">
         <v>38</v>
@@ -1122,8 +1158,10 @@
       <c r="N19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>95</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
       </c>
       <c r="B20" t="n">
         <v>20</v>
@@ -1158,8 +1196,10 @@
       <c r="N20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>95</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
       </c>
       <c r="B21" t="n">
         <v>10</v>
@@ -1194,8 +1234,10 @@
       <c r="N21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>95</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
       </c>
       <c r="B22" t="n">
         <v>2</v>
@@ -1230,8 +1272,10 @@
       <c r="N22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>95</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
       </c>
       <c r="B23" t="n">
         <v>25</v>
@@ -1266,8 +1310,10 @@
       <c r="N23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>106</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
       </c>
       <c r="B24" t="n">
         <v>38</v>
@@ -1302,8 +1348,10 @@
       <c r="N24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>106</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
       </c>
       <c r="B25" t="n">
         <v>20</v>
@@ -1338,8 +1386,10 @@
       <c r="N25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>106</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
       </c>
       <c r="B26" t="n">
         <v>10</v>
@@ -1374,8 +1424,10 @@
       <c r="N26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>106</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
       </c>
       <c r="B27" t="n">
         <v>2</v>
@@ -1410,8 +1462,10 @@
       <c r="N27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>106</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
       </c>
       <c r="B28" t="n">
         <v>25</v>
@@ -1446,8 +1500,10 @@
       <c r="N28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>113</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
       </c>
       <c r="B29" t="n">
         <v>42</v>
@@ -1482,8 +1538,10 @@
       <c r="N29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>113</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
       </c>
       <c r="B30" t="n">
         <v>20</v>
@@ -1518,8 +1576,10 @@
       <c r="N30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>113</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
       </c>
       <c r="B31" t="n">
         <v>10</v>
@@ -1554,8 +1614,10 @@
       <c r="N31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>113</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
       </c>
       <c r="B32" t="n">
         <v>2</v>
@@ -1590,8 +1652,10 @@
       <c r="N32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>113</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
       </c>
       <c r="B33" t="n">
         <v>25</v>
@@ -1626,8 +1690,10 @@
       <c r="N33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>118</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
       </c>
       <c r="B34" t="n">
         <v>58</v>
@@ -1662,8 +1728,10 @@
       <c r="N34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>118</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
       </c>
       <c r="B35" t="n">
         <v>40</v>
@@ -1698,8 +1766,10 @@
       <c r="N35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>118</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
       </c>
       <c r="B36" t="n">
         <v>20</v>
@@ -1734,8 +1804,10 @@
       <c r="N36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>118</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
       </c>
       <c r="B37" t="n">
         <v>10</v>
@@ -1770,8 +1842,10 @@
       <c r="N37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>118</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
       </c>
       <c r="B38" t="n">
         <v>2</v>
@@ -1806,8 +1880,10 @@
       <c r="N38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>118</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
       </c>
       <c r="B39" t="n">
         <v>25</v>
@@ -1842,8 +1918,10 @@
       <c r="N39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>127</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
       </c>
       <c r="B40" t="n">
         <v>88</v>
@@ -1878,8 +1956,10 @@
       <c r="N40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>127</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
       </c>
       <c r="B41" t="n">
         <v>40</v>
@@ -1914,8 +1994,10 @@
       <c r="N41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>127</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
       </c>
       <c r="B42" t="n">
         <v>20</v>
@@ -1950,8 +2032,10 @@
       <c r="N42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>127</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
       </c>
       <c r="B43" t="n">
         <v>10</v>
@@ -1986,8 +2070,10 @@
       <c r="N43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>127</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
       </c>
       <c r="B44" t="n">
         <v>2</v>
@@ -2022,8 +2108,10 @@
       <c r="N44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>127</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
       </c>
       <c r="B45" t="n">
         <v>25</v>
@@ -2058,8 +2146,10 @@
       <c r="N45" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>133</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>133</t>
+        </is>
       </c>
       <c r="B46" t="n">
         <v>120</v>
@@ -2094,8 +2184,10 @@
       <c r="N46" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>133</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>133</t>
+        </is>
       </c>
       <c r="B47" t="n">
         <v>40</v>
@@ -2130,8 +2222,10 @@
       <c r="N47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>133</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>133</t>
+        </is>
       </c>
       <c r="B48" t="n">
         <v>20</v>
@@ -2166,8 +2260,10 @@
       <c r="N48" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>133</v>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>133</t>
+        </is>
       </c>
       <c r="B49" t="n">
         <v>10</v>
@@ -2202,8 +2298,10 @@
       <c r="N49" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>133</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>133</t>
+        </is>
       </c>
       <c r="B50" t="n">
         <v>2</v>
@@ -2222,8 +2320,10 @@
       <c r="N50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>133</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>133</t>
+        </is>
       </c>
       <c r="B51" t="n">
         <v>25</v>

</xml_diff>